<commit_message>
add notify for dangky and monhoc
</commit_message>
<xml_diff>
--- a/database/data_lophp.xlsx
+++ b/database/data_lophp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DangKyHocPhan\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62EAAF3-9172-4221-8D84-18CC9465D120}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3883D01D-2E6A-45F5-AE0F-BC1482B63215}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9684" xr2:uid="{D1BFA2C3-3278-40ED-B2F9-F11C83CA4857}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
add notify for all admin view
</commit_message>
<xml_diff>
--- a/database/data_lophp.xlsx
+++ b/database/data_lophp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DangKyHocPhan\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3883D01D-2E6A-45F5-AE0F-BC1482B63215}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005B5BE0-3EDF-4E32-902B-DFC25DD67702}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9684" xr2:uid="{D1BFA2C3-3278-40ED-B2F9-F11C83CA4857}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>mamh</t>
   </si>
   <si>
-    <t>LHP001</t>
-  </si>
-  <si>
     <t>Hệ thống nhúng-L01</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>MH001</t>
   </si>
   <si>
-    <t>LHP002</t>
-  </si>
-  <si>
     <t>Hệ thống nhúng-L02</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
     <t>GV006</t>
   </si>
   <si>
-    <t>LHP003</t>
-  </si>
-  <si>
     <t>Thứ 2 - Tiết 4,5,6</t>
   </si>
   <si>
@@ -96,30 +87,12 @@
     <t>MH003</t>
   </si>
   <si>
-    <t>LHP004</t>
-  </si>
-  <si>
-    <t>LHP005</t>
-  </si>
-  <si>
     <t>Thứ 3 - Tiết 1,2,3</t>
   </si>
   <si>
     <t>MH005</t>
   </si>
   <si>
-    <t>LHP006</t>
-  </si>
-  <si>
-    <t>LHP007</t>
-  </si>
-  <si>
-    <t>LHP008</t>
-  </si>
-  <si>
-    <t>LHP009</t>
-  </si>
-  <si>
     <t>Kiến trúc máy tính-L01</t>
   </si>
   <si>
@@ -159,15 +132,6 @@
     <t>GV005</t>
   </si>
   <si>
-    <t>LHP010</t>
-  </si>
-  <si>
-    <t>LHP011</t>
-  </si>
-  <si>
-    <t>LHP012</t>
-  </si>
-  <si>
     <t>Đại số tuyến tính-L01</t>
   </si>
   <si>
@@ -198,13 +162,49 @@
     <t>Phòng B304</t>
   </si>
   <si>
-    <t>LHP013</t>
-  </si>
-  <si>
     <t>KT chế tạo vô tuyến-L01</t>
   </si>
   <si>
     <t>MH012</t>
+  </si>
+  <si>
+    <t>MH001-LHP001</t>
+  </si>
+  <si>
+    <t>MH001-LHP002</t>
+  </si>
+  <si>
+    <t>MH003-LHP001</t>
+  </si>
+  <si>
+    <t>MH003-LHP002</t>
+  </si>
+  <si>
+    <t>MH005-LHP001</t>
+  </si>
+  <si>
+    <t>MH005-LHP002</t>
+  </si>
+  <si>
+    <t>MH007-LHP002</t>
+  </si>
+  <si>
+    <t>MH007-LHP001</t>
+  </si>
+  <si>
+    <t>MH009-LHP001</t>
+  </si>
+  <si>
+    <t>MH009-LHP002</t>
+  </si>
+  <si>
+    <t>MH011-LHP001</t>
+  </si>
+  <si>
+    <t>MH011-LHP002</t>
+  </si>
+  <si>
+    <t>MH012-LHP001</t>
   </si>
 </sst>
 </file>
@@ -568,7 +568,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -608,301 +608,301 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="C6" s="1">
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>